<commit_message>
Rxn Network filled rate coefficients
</commit_message>
<xml_diff>
--- a/Earth-Inputs/REACTION_NETWORK_EARTH.xlsx
+++ b/Earth-Inputs/REACTION_NETWORK_EARTH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pbt92\Documents\GitHub\bluejay\Earth-Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ebenezersolomon/Documents/GitHub/bluejay/Earth-Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47FD0E0-6F44-4646-BF1F-FFFCF99FFB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96B9AAE-7B96-E947-93D7-3730149D10FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="3" xr2:uid="{F49DAA0A-82A3-4B5F-9C2C-4D9969D3062E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F49DAA0A-82A3-4B5F-9C2C-4D9969D3062E}"/>
   </bookViews>
   <sheets>
     <sheet name="Neutral reactions" sheetId="2" r:id="rId1"/>
@@ -671,13 +671,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B54FE042-F072-4117-BA7D-F060653EB408}">
   <dimension ref="A1:Y116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AB29" sqref="AB29"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="V116" sqref="V116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -754,7 +754,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -816,7 +816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -848,7 +848,13 @@
         <v>0</v>
       </c>
       <c r="L3" s="1">
-        <v>2.1999999999999999E-10</v>
+        <v>1.2400000000000001E-10</v>
+      </c>
+      <c r="M3">
+        <v>0.26</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
       </c>
       <c r="O3">
         <v>0</v>
@@ -872,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -906,6 +912,12 @@
       <c r="L4" s="1">
         <v>2.1999999999999999E-10</v>
       </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0.32</v>
+      </c>
       <c r="O4">
         <v>0</v>
       </c>
@@ -928,7 +940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -990,7 +1002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1052,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1114,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -1148,6 +1160,15 @@
       <c r="K8">
         <v>0.5</v>
       </c>
+      <c r="L8" s="1">
+        <v>3.1000000000000002E-10</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1650</v>
+      </c>
       <c r="O8">
         <v>0</v>
       </c>
@@ -1170,7 +1191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1204,6 +1225,15 @@
       <c r="K9">
         <v>0.5</v>
       </c>
+      <c r="L9" s="1">
+        <v>2.0000000000000001E-10</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
       <c r="O9">
         <v>0</v>
       </c>
@@ -1226,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1257,6 +1287,15 @@
       <c r="J10">
         <v>0</v>
       </c>
+      <c r="L10" s="1">
+        <v>1.9999999999999999E-11</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
       <c r="O10">
         <v>0</v>
       </c>
@@ -1279,7 +1318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -1313,6 +1352,15 @@
       <c r="K11">
         <v>0.5</v>
       </c>
+      <c r="L11" s="1">
+        <v>2.0000000000000001E-10</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
       <c r="O11">
         <v>0</v>
       </c>
@@ -1335,7 +1383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1369,6 +1417,15 @@
       <c r="K12">
         <v>0.5</v>
       </c>
+      <c r="L12" s="1">
+        <v>9.9999999999999994E-12</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
       <c r="O12">
         <v>0</v>
       </c>
@@ -1391,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -1453,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -1515,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -1580,7 +1637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -1645,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -1710,7 +1767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1775,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -1837,7 +1894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1899,7 +1956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1961,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -2023,7 +2080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -2085,7 +2142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -2150,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -2215,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -2280,7 +2337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -2345,7 +2402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2407,7 +2464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -2469,7 +2526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -2534,7 +2591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -2599,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -2630,6 +2687,15 @@
       <c r="J32">
         <v>0</v>
       </c>
+      <c r="L32" s="1">
+        <v>4.9999999999999997E-12</v>
+      </c>
+      <c r="M32" s="1">
+        <v>0</v>
+      </c>
+      <c r="N32" s="1">
+        <v>0</v>
+      </c>
       <c r="O32">
         <v>0</v>
       </c>
@@ -2652,7 +2718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -2714,7 +2780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -2776,7 +2842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -2838,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -2900,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2931,6 +2997,15 @@
       <c r="J37">
         <v>0</v>
       </c>
+      <c r="L37" s="1">
+        <v>1E-13</v>
+      </c>
+      <c r="M37" s="1">
+        <v>0</v>
+      </c>
+      <c r="N37" s="1">
+        <v>520</v>
+      </c>
       <c r="O37">
         <v>0</v>
       </c>
@@ -2953,7 +3028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -2984,6 +3059,15 @@
       <c r="J38">
         <v>0</v>
       </c>
+      <c r="L38" s="1">
+        <v>5.0000000000000002E-11</v>
+      </c>
+      <c r="M38" s="1">
+        <v>0</v>
+      </c>
+      <c r="N38" s="1">
+        <v>0</v>
+      </c>
       <c r="O38">
         <v>0</v>
       </c>
@@ -3006,7 +3090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -3037,6 +3121,15 @@
       <c r="J39">
         <v>0</v>
       </c>
+      <c r="L39" s="1">
+        <v>5.0000000000000002E-11</v>
+      </c>
+      <c r="M39" s="1">
+        <v>0</v>
+      </c>
+      <c r="N39" s="1">
+        <v>0</v>
+      </c>
       <c r="O39">
         <v>0</v>
       </c>
@@ -3059,7 +3152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -3121,7 +3214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -3186,7 +3279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -3251,7 +3344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -3316,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -3381,7 +3474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -3446,7 +3539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -3508,7 +3601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -3570,7 +3663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -3601,6 +3694,15 @@
       <c r="J48">
         <v>0</v>
       </c>
+      <c r="L48" s="1">
+        <v>2.0000000000000001E-10</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
       <c r="O48">
         <v>0</v>
       </c>
@@ -3623,7 +3725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -3654,6 +3756,15 @@
       <c r="J49">
         <v>0</v>
       </c>
+      <c r="L49" s="1">
+        <v>1E-10</v>
+      </c>
+      <c r="M49">
+        <v>0.17</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
       <c r="O49">
         <v>0</v>
       </c>
@@ -3676,7 +3787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>46</v>
       </c>
@@ -3707,6 +3818,15 @@
       <c r="J50">
         <v>0</v>
       </c>
+      <c r="L50" s="1">
+        <v>1E-10</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
       <c r="O50">
         <v>0</v>
       </c>
@@ -3729,7 +3849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>46</v>
       </c>
@@ -3791,7 +3911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -3853,7 +3973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -3915,7 +4035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -3977,7 +4097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -4008,6 +4128,15 @@
       <c r="J55">
         <v>0</v>
       </c>
+      <c r="L55" s="1">
+        <v>1.1099999999999999E-13</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55" s="1">
+        <v>-1850</v>
+      </c>
       <c r="O55">
         <v>0</v>
       </c>
@@ -4030,7 +4159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -4061,6 +4190,15 @@
       <c r="J56">
         <v>0</v>
       </c>
+      <c r="L56" s="1">
+        <v>1.9999999999999999E-11</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56" s="1">
+        <v>0</v>
+      </c>
       <c r="O56">
         <v>0</v>
       </c>
@@ -4083,7 +4221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -4145,7 +4283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>68</v>
       </c>
@@ -4207,7 +4345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -4269,7 +4407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -4331,7 +4469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>49</v>
       </c>
@@ -4362,6 +4500,15 @@
       <c r="J61">
         <v>0</v>
       </c>
+      <c r="L61" s="1">
+        <v>4.1200000000000001E-13</v>
+      </c>
+      <c r="M61" s="1">
+        <v>2.87</v>
+      </c>
+      <c r="N61" s="1">
+        <v>-820</v>
+      </c>
       <c r="O61">
         <v>0</v>
       </c>
@@ -4384,7 +4531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>49</v>
       </c>
@@ -4449,7 +4596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>49</v>
       </c>
@@ -4483,6 +4630,15 @@
       <c r="K63">
         <v>0.33</v>
       </c>
+      <c r="L63" s="1">
+        <v>5.0000000000000002E-11</v>
+      </c>
+      <c r="M63" s="1">
+        <v>0</v>
+      </c>
+      <c r="N63" s="1">
+        <v>0</v>
+      </c>
       <c r="O63">
         <v>0</v>
       </c>
@@ -4505,7 +4661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>49</v>
       </c>
@@ -4539,6 +4695,15 @@
       <c r="K64">
         <v>0.33</v>
       </c>
+      <c r="L64" s="1">
+        <v>5.0000000000000002E-11</v>
+      </c>
+      <c r="M64" s="1">
+        <v>0</v>
+      </c>
+      <c r="N64" s="1">
+        <v>0</v>
+      </c>
       <c r="O64">
         <v>0</v>
       </c>
@@ -4561,7 +4726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>49</v>
       </c>
@@ -4623,7 +4788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>49</v>
       </c>
@@ -4685,7 +4850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>49</v>
       </c>
@@ -4747,7 +4912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>49</v>
       </c>
@@ -4809,7 +4974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>49</v>
       </c>
@@ -4840,6 +5005,15 @@
       <c r="J69">
         <v>0</v>
       </c>
+      <c r="L69" s="1">
+        <v>4.2999999999999999E-13</v>
+      </c>
+      <c r="M69" s="1">
+        <v>1.71</v>
+      </c>
+      <c r="N69" s="1">
+        <v>-770</v>
+      </c>
       <c r="O69">
         <v>0</v>
       </c>
@@ -4862,7 +5036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>49</v>
       </c>
@@ -4927,7 +5101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>56</v>
       </c>
@@ -4992,7 +5166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>56</v>
       </c>
@@ -5054,7 +5228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>56</v>
       </c>
@@ -5116,7 +5290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>65</v>
       </c>
@@ -5178,7 +5352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>66</v>
       </c>
@@ -5209,6 +5383,15 @@
       <c r="J75">
         <v>0</v>
       </c>
+      <c r="L75" s="1">
+        <v>6E-11</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="N75" s="1">
+        <v>0</v>
+      </c>
       <c r="O75">
         <v>0</v>
       </c>
@@ -5231,7 +5414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>66</v>
       </c>
@@ -5293,7 +5476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>53</v>
       </c>
@@ -5355,7 +5538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>53</v>
       </c>
@@ -5417,7 +5600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>53</v>
       </c>
@@ -5479,7 +5662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>53</v>
       </c>
@@ -5541,7 +5724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>53</v>
       </c>
@@ -5603,7 +5786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>53</v>
       </c>
@@ -5665,7 +5848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>53</v>
       </c>
@@ -5727,7 +5910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>53</v>
       </c>
@@ -5789,7 +5972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>53</v>
       </c>
@@ -5851,7 +6034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>53</v>
       </c>
@@ -5913,7 +6096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>78</v>
       </c>
@@ -5978,7 +6161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>78</v>
       </c>
@@ -6012,6 +6195,15 @@
       <c r="K88">
         <v>0.33</v>
       </c>
+      <c r="L88" s="1">
+        <v>1.05E-10</v>
+      </c>
+      <c r="M88">
+        <v>0</v>
+      </c>
+      <c r="N88" s="1">
+        <v>0</v>
+      </c>
       <c r="O88">
         <v>0</v>
       </c>
@@ -6034,7 +6226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>78</v>
       </c>
@@ -6099,7 +6291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>78</v>
       </c>
@@ -6161,7 +6353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>78</v>
       </c>
@@ -6223,7 +6415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>32</v>
       </c>
@@ -6285,7 +6477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>32</v>
       </c>
@@ -6347,7 +6539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>32</v>
       </c>
@@ -6409,7 +6601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>32</v>
       </c>
@@ -6471,7 +6663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>32</v>
       </c>
@@ -6533,7 +6725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>34</v>
       </c>
@@ -6598,7 +6790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>34</v>
       </c>
@@ -6632,6 +6824,15 @@
       <c r="K98">
         <v>0.5</v>
       </c>
+      <c r="L98" s="1">
+        <v>4.9999999999999997E-12</v>
+      </c>
+      <c r="M98">
+        <v>0</v>
+      </c>
+      <c r="N98" s="1">
+        <v>0</v>
+      </c>
       <c r="O98">
         <v>0</v>
       </c>
@@ -6654,7 +6855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>34</v>
       </c>
@@ -6716,7 +6917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>43</v>
       </c>
@@ -6747,9 +6948,6 @@
       <c r="J100">
         <v>0</v>
       </c>
-      <c r="K100">
-        <v>0.25</v>
-      </c>
       <c r="L100" s="1">
         <v>1.3100000000000001E-10</v>
       </c>
@@ -6781,7 +6979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>40</v>
       </c>
@@ -6846,7 +7044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>40</v>
       </c>
@@ -6911,7 +7109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>40</v>
       </c>
@@ -6976,7 +7174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>40</v>
       </c>
@@ -7008,7 +7206,16 @@
         <v>0</v>
       </c>
       <c r="K104">
-        <v>0.5</v>
+        <v>0.25</v>
+      </c>
+      <c r="L104" s="1">
+        <v>9.9999999999999994E-12</v>
+      </c>
+      <c r="M104">
+        <v>-0.13</v>
+      </c>
+      <c r="N104" s="1">
+        <v>0</v>
       </c>
       <c r="O104">
         <v>0</v>
@@ -7032,7 +7239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>40</v>
       </c>
@@ -7066,6 +7273,15 @@
       <c r="K105">
         <v>0.5</v>
       </c>
+      <c r="L105" s="1">
+        <v>2.0999999999999999E-12</v>
+      </c>
+      <c r="M105">
+        <v>0</v>
+      </c>
+      <c r="N105" s="1">
+        <v>554</v>
+      </c>
       <c r="O105">
         <v>0</v>
       </c>
@@ -7088,7 +7304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>40</v>
       </c>
@@ -7119,6 +7335,18 @@
       <c r="J106">
         <v>0</v>
       </c>
+      <c r="K106">
+        <v>0.5</v>
+      </c>
+      <c r="L106" s="1">
+        <v>2.9999999999999998E-13</v>
+      </c>
+      <c r="M106">
+        <v>0</v>
+      </c>
+      <c r="N106" s="1">
+        <v>554</v>
+      </c>
       <c r="O106">
         <v>0</v>
       </c>
@@ -7141,7 +7369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>40</v>
       </c>
@@ -7172,6 +7400,15 @@
       <c r="J107">
         <v>0</v>
       </c>
+      <c r="L107" s="1">
+        <v>3.9999999999999998E-11</v>
+      </c>
+      <c r="M107">
+        <v>0</v>
+      </c>
+      <c r="N107" s="1">
+        <v>0</v>
+      </c>
       <c r="O107">
         <v>0</v>
       </c>
@@ -7194,7 +7431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>40</v>
       </c>
@@ -7225,6 +7462,15 @@
       <c r="J108">
         <v>0</v>
       </c>
+      <c r="L108" s="1">
+        <v>6E-11</v>
+      </c>
+      <c r="M108">
+        <v>0</v>
+      </c>
+      <c r="N108" s="1">
+        <v>0</v>
+      </c>
       <c r="O108">
         <v>0</v>
       </c>
@@ -7247,7 +7493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>40</v>
       </c>
@@ -7278,6 +7524,15 @@
       <c r="J109">
         <v>0</v>
       </c>
+      <c r="L109" s="1">
+        <v>2.9E-11</v>
+      </c>
+      <c r="M109">
+        <v>-0.3</v>
+      </c>
+      <c r="N109" s="1">
+        <v>77</v>
+      </c>
       <c r="O109">
         <v>0</v>
       </c>
@@ -7300,7 +7555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>40</v>
       </c>
@@ -7362,7 +7617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>47</v>
       </c>
@@ -7393,6 +7648,15 @@
       <c r="J111">
         <v>0</v>
       </c>
+      <c r="L111" s="1">
+        <v>5.0000000000000002E-11</v>
+      </c>
+      <c r="M111">
+        <v>0</v>
+      </c>
+      <c r="N111" s="1">
+        <v>0</v>
+      </c>
       <c r="O111">
         <v>0</v>
       </c>
@@ -7415,7 +7679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>55</v>
       </c>
@@ -7446,6 +7710,15 @@
       <c r="J112">
         <v>0</v>
       </c>
+      <c r="L112" s="1">
+        <v>1.5E-11</v>
+      </c>
+      <c r="M112">
+        <v>0</v>
+      </c>
+      <c r="N112" s="1">
+        <v>257</v>
+      </c>
       <c r="O112">
         <v>0</v>
       </c>
@@ -7468,7 +7741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>55</v>
       </c>
@@ -7530,7 +7803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>35</v>
       </c>
@@ -7561,6 +7834,15 @@
       <c r="J114">
         <v>0</v>
       </c>
+      <c r="L114" s="1">
+        <v>9.1399999999999995E-33</v>
+      </c>
+      <c r="M114">
+        <v>-0.6</v>
+      </c>
+      <c r="N114" s="1">
+        <v>0</v>
+      </c>
       <c r="O114">
         <v>0</v>
       </c>
@@ -7583,7 +7865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>35</v>
       </c>
@@ -7614,6 +7896,15 @@
       <c r="J115">
         <v>0</v>
       </c>
+      <c r="L115" s="1">
+        <v>8.9000000000000002E-29</v>
+      </c>
+      <c r="M115">
+        <v>-0.18</v>
+      </c>
+      <c r="N115" s="1">
+        <v>-31.8</v>
+      </c>
       <c r="O115">
         <v>0</v>
       </c>
@@ -7636,7 +7927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>56</v>
       </c>
@@ -7665,6 +7956,36 @@
         <v>1</v>
       </c>
       <c r="J116">
+        <v>0</v>
+      </c>
+      <c r="L116" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="M116">
+        <v>0</v>
+      </c>
+      <c r="N116" s="1">
+        <v>-2080</v>
+      </c>
+      <c r="O116">
+        <v>0</v>
+      </c>
+      <c r="P116" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q116">
+        <v>0</v>
+      </c>
+      <c r="R116" s="1">
+        <v>0</v>
+      </c>
+      <c r="S116">
+        <v>0</v>
+      </c>
+      <c r="T116" s="1">
+        <v>0</v>
+      </c>
+      <c r="U116">
         <v>0</v>
       </c>
     </row>
@@ -7681,9 +8002,9 @@
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7794,9 +8115,9 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7873,13 +8194,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF76566-3451-4152-A8DD-AC31325D9527}">
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
C2H2 and C2H4 Photodissociation
</commit_message>
<xml_diff>
--- a/Earth-Inputs/REACTION_NETWORK_EARTH.xlsx
+++ b/Earth-Inputs/REACTION_NETWORK_EARTH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pbt92\Documents\GitHub\bluejay\Earth-Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204080CC-FF49-4003-96A8-596FD870AEBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF691D8-5EF0-4F4D-93A8-3268215872A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="5280" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Neutral reactions" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,19 @@
     <sheet name="Photodissociation" sheetId="3" r:id="rId3"/>
     <sheet name="Photoionization" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -28,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6513" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6555" uniqueCount="253">
   <si>
     <t>R1</t>
   </si>
@@ -770,6 +781,24 @@
   <si>
     <t>New</t>
   </si>
+  <si>
+    <t xml:space="preserve">none </t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>296 K</t>
+  </si>
+  <si>
+    <t>Stubbing 2015</t>
+  </si>
+  <si>
+    <t>Balancing Airapetian Network</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ebenezer Solomon </t>
+  </si>
 </sst>
 </file>
 
@@ -1164,8 +1193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y440"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG20" sqref="AG20"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M86" sqref="M86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1267,7 +1296,7 @@
         <v>78</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1329,7 +1358,7 @@
         <v>78</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1391,7 +1420,7 @@
         <v>78</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1453,7 +1482,7 @@
         <v>78</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1515,7 +1544,7 @@
         <v>78</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1577,7 +1606,7 @@
         <v>78</v>
       </c>
       <c r="G7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -1642,7 +1671,7 @@
         <v>78</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1707,7 +1736,7 @@
         <v>78</v>
       </c>
       <c r="G9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1772,7 +1801,7 @@
         <v>78</v>
       </c>
       <c r="G10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1837,7 +1866,7 @@
         <v>31</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -1899,7 +1928,7 @@
         <v>78</v>
       </c>
       <c r="G12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -1961,7 +1990,7 @@
         <v>78</v>
       </c>
       <c r="G13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2023,7 +2052,7 @@
         <v>78</v>
       </c>
       <c r="G14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -2088,7 +2117,7 @@
         <v>78</v>
       </c>
       <c r="G15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -2153,7 +2182,7 @@
         <v>78</v>
       </c>
       <c r="G16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2218,7 +2247,7 @@
         <v>78</v>
       </c>
       <c r="G17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -2283,7 +2312,7 @@
         <v>78</v>
       </c>
       <c r="G18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -2345,7 +2374,7 @@
         <v>78</v>
       </c>
       <c r="G19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2407,7 +2436,7 @@
         <v>78</v>
       </c>
       <c r="G20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2469,7 +2498,7 @@
         <v>78</v>
       </c>
       <c r="G21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -2531,7 +2560,7 @@
         <v>78</v>
       </c>
       <c r="G22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2596,7 +2625,7 @@
         <v>78</v>
       </c>
       <c r="G23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2661,7 +2690,7 @@
         <v>78</v>
       </c>
       <c r="G24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -2726,7 +2755,7 @@
         <v>78</v>
       </c>
       <c r="G25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -2791,7 +2820,7 @@
         <v>31</v>
       </c>
       <c r="G26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -2853,7 +2882,7 @@
         <v>78</v>
       </c>
       <c r="G27">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -2915,7 +2944,7 @@
         <v>78</v>
       </c>
       <c r="G28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -2980,7 +3009,7 @@
         <v>78</v>
       </c>
       <c r="G29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -3036,7 +3065,7 @@
         <v>78</v>
       </c>
       <c r="G30">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H30">
         <v>1</v>
@@ -3098,7 +3127,7 @@
         <v>78</v>
       </c>
       <c r="G31">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -3160,7 +3189,7 @@
         <v>78</v>
       </c>
       <c r="G32">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -3222,7 +3251,7 @@
         <v>78</v>
       </c>
       <c r="G33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -3284,7 +3313,7 @@
         <v>78</v>
       </c>
       <c r="G34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -3346,7 +3375,7 @@
         <v>78</v>
       </c>
       <c r="G35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H35">
         <v>1</v>
@@ -3408,7 +3437,7 @@
         <v>78</v>
       </c>
       <c r="G36">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -3470,7 +3499,7 @@
         <v>78</v>
       </c>
       <c r="G37">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H37">
         <v>1</v>
@@ -3532,7 +3561,7 @@
         <v>78</v>
       </c>
       <c r="G38">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -3597,7 +3626,7 @@
         <v>78</v>
       </c>
       <c r="G39">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -3662,7 +3691,7 @@
         <v>78</v>
       </c>
       <c r="G40">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -3727,7 +3756,7 @@
         <v>78</v>
       </c>
       <c r="G41">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -3792,7 +3821,7 @@
         <v>31</v>
       </c>
       <c r="G42">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -3857,7 +3886,7 @@
         <v>78</v>
       </c>
       <c r="G43">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -3919,7 +3948,7 @@
         <v>78</v>
       </c>
       <c r="G44">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -3981,7 +4010,7 @@
         <v>31</v>
       </c>
       <c r="G45">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -4043,7 +4072,7 @@
         <v>78</v>
       </c>
       <c r="G46">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H46">
         <v>1</v>
@@ -4105,7 +4134,7 @@
         <v>78</v>
       </c>
       <c r="G47">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H47">
         <v>1</v>
@@ -4167,7 +4196,7 @@
         <v>78</v>
       </c>
       <c r="G48">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H48">
         <v>1</v>
@@ -4229,7 +4258,7 @@
         <v>78</v>
       </c>
       <c r="G49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H49">
         <v>1</v>
@@ -4291,7 +4320,7 @@
         <v>78</v>
       </c>
       <c r="G50">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H50">
         <v>1</v>
@@ -4353,7 +4382,7 @@
         <v>78</v>
       </c>
       <c r="G51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H51">
         <v>1</v>
@@ -4415,7 +4444,7 @@
         <v>78</v>
       </c>
       <c r="G52">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -4477,7 +4506,7 @@
         <v>78</v>
       </c>
       <c r="G53">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -4539,7 +4568,7 @@
         <v>78</v>
       </c>
       <c r="G54">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H54">
         <v>1</v>
@@ -4601,7 +4630,7 @@
         <v>78</v>
       </c>
       <c r="G55">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -4663,7 +4692,7 @@
         <v>78</v>
       </c>
       <c r="G56">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -4725,7 +4754,7 @@
         <v>78</v>
       </c>
       <c r="G57">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -4787,7 +4816,7 @@
         <v>78</v>
       </c>
       <c r="G58">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H58">
         <v>1</v>
@@ -4849,7 +4878,7 @@
         <v>78</v>
       </c>
       <c r="G59">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -4914,7 +4943,7 @@
         <v>78</v>
       </c>
       <c r="G60">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -4979,7 +5008,7 @@
         <v>78</v>
       </c>
       <c r="G61">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -5041,7 +5070,7 @@
         <v>78</v>
       </c>
       <c r="G62">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H62">
         <v>1</v>
@@ -5103,7 +5132,7 @@
         <v>78</v>
       </c>
       <c r="G63">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H63">
         <v>1</v>
@@ -5165,7 +5194,7 @@
         <v>78</v>
       </c>
       <c r="G64">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H64">
         <v>1</v>
@@ -5227,7 +5256,7 @@
         <v>78</v>
       </c>
       <c r="G65">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -5289,7 +5318,7 @@
         <v>78</v>
       </c>
       <c r="G66">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -5354,7 +5383,7 @@
         <v>78</v>
       </c>
       <c r="G67">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -5419,7 +5448,7 @@
         <v>78</v>
       </c>
       <c r="G68">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H68">
         <v>1</v>
@@ -5481,7 +5510,7 @@
         <v>78</v>
       </c>
       <c r="G69">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H69">
         <v>1</v>
@@ -5543,7 +5572,7 @@
         <v>78</v>
       </c>
       <c r="G70">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H70">
         <v>1</v>
@@ -5605,7 +5634,7 @@
         <v>78</v>
       </c>
       <c r="G71">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -5667,7 +5696,7 @@
         <v>78</v>
       </c>
       <c r="G72">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -5729,7 +5758,7 @@
         <v>31</v>
       </c>
       <c r="G73">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -5791,7 +5820,7 @@
         <v>78</v>
       </c>
       <c r="G74">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -5853,7 +5882,7 @@
         <v>78</v>
       </c>
       <c r="G75">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H75">
         <v>1</v>
@@ -5915,7 +5944,7 @@
         <v>31</v>
       </c>
       <c r="G76">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H76">
         <v>1</v>
@@ -5977,7 +6006,7 @@
         <v>78</v>
       </c>
       <c r="G77">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -6039,7 +6068,7 @@
         <v>31</v>
       </c>
       <c r="G78">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -6101,7 +6130,7 @@
         <v>78</v>
       </c>
       <c r="G79">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -6163,7 +6192,7 @@
         <v>78</v>
       </c>
       <c r="G80">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -6225,7 +6254,7 @@
         <v>78</v>
       </c>
       <c r="G81">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H81">
         <v>1</v>
@@ -6287,7 +6316,7 @@
         <v>78</v>
       </c>
       <c r="G82">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -6352,7 +6381,7 @@
         <v>78</v>
       </c>
       <c r="G83">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -6417,7 +6446,7 @@
         <v>78</v>
       </c>
       <c r="G84">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H84">
         <v>1</v>
@@ -6482,7 +6511,7 @@
         <v>78</v>
       </c>
       <c r="G85">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -6544,7 +6573,7 @@
         <v>78</v>
       </c>
       <c r="G86">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H86">
         <v>1</v>
@@ -6606,7 +6635,7 @@
         <v>78</v>
       </c>
       <c r="G87">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H87">
         <v>1</v>
@@ -6668,7 +6697,7 @@
         <v>78</v>
       </c>
       <c r="G88">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H88">
         <v>1</v>
@@ -6730,7 +6759,7 @@
         <v>78</v>
       </c>
       <c r="G89">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H89">
         <v>1</v>
@@ -6792,7 +6821,7 @@
         <v>78</v>
       </c>
       <c r="G90">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H90">
         <v>1</v>
@@ -6854,7 +6883,7 @@
         <v>78</v>
       </c>
       <c r="G91">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -6916,7 +6945,7 @@
         <v>78</v>
       </c>
       <c r="G92">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H92">
         <v>1</v>
@@ -6981,7 +7010,7 @@
         <v>78</v>
       </c>
       <c r="G93">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H93">
         <v>1</v>
@@ -7046,7 +7075,7 @@
         <v>78</v>
       </c>
       <c r="G94">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H94">
         <v>1</v>
@@ -7108,7 +7137,7 @@
         <v>78</v>
       </c>
       <c r="G95">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H95">
         <v>1</v>
@@ -7170,7 +7199,7 @@
         <v>78</v>
       </c>
       <c r="G96">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H96">
         <v>1</v>
@@ -7215,7 +7244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>47</v>
       </c>
@@ -7235,7 +7264,7 @@
         <v>78</v>
       </c>
       <c r="G97">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H97">
         <v>1</v>
@@ -7280,7 +7309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>47</v>
       </c>
@@ -7300,7 +7329,7 @@
         <v>78</v>
       </c>
       <c r="G98">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H98">
         <v>1</v>
@@ -7345,7 +7374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>47</v>
       </c>
@@ -7365,7 +7394,7 @@
         <v>78</v>
       </c>
       <c r="G99">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H99">
         <v>1</v>
@@ -7410,7 +7439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>47</v>
       </c>
@@ -7430,7 +7459,7 @@
         <v>78</v>
       </c>
       <c r="G100">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H100">
         <v>1</v>
@@ -7475,7 +7504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>47</v>
       </c>
@@ -7495,7 +7524,7 @@
         <v>78</v>
       </c>
       <c r="G101">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H101">
         <v>1</v>
@@ -7540,7 +7569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>47</v>
       </c>
@@ -7560,7 +7589,7 @@
         <v>78</v>
       </c>
       <c r="G102">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H102">
         <v>1</v>
@@ -7602,7 +7631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>47</v>
       </c>
@@ -7622,7 +7651,7 @@
         <v>78</v>
       </c>
       <c r="G103">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H103">
         <v>1</v>
@@ -7664,7 +7693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>47</v>
       </c>
@@ -7684,7 +7713,7 @@
         <v>78</v>
       </c>
       <c r="G104">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H104">
         <v>1</v>
@@ -7726,7 +7755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>47</v>
       </c>
@@ -7746,7 +7775,7 @@
         <v>78</v>
       </c>
       <c r="G105">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H105">
         <v>1</v>
@@ -7788,7 +7817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>60</v>
       </c>
@@ -7808,7 +7837,7 @@
         <v>78</v>
       </c>
       <c r="G106">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H106">
         <v>1</v>
@@ -7850,7 +7879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>62</v>
       </c>
@@ -7870,7 +7899,7 @@
         <v>78</v>
       </c>
       <c r="G107">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H107">
         <v>1</v>
@@ -7912,7 +7941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>62</v>
       </c>
@@ -7932,7 +7961,7 @@
         <v>78</v>
       </c>
       <c r="G108">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H108">
         <v>1</v>
@@ -7974,7 +8003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>31</v>
       </c>
@@ -7994,7 +8023,7 @@
         <v>78</v>
       </c>
       <c r="G109">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H109">
         <v>1</v>
@@ -8036,7 +8065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>31</v>
       </c>
@@ -8056,7 +8085,7 @@
         <v>78</v>
       </c>
       <c r="G110">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H110">
         <v>1</v>
@@ -8098,7 +8127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>44</v>
       </c>
@@ -8118,7 +8147,7 @@
         <v>78</v>
       </c>
       <c r="G111">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H111">
         <v>1</v>
@@ -8158,6 +8187,80 @@
       </c>
       <c r="U111">
         <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>229</v>
+      </c>
+      <c r="B112" t="s">
+        <v>235</v>
+      </c>
+      <c r="C112" t="s">
+        <v>78</v>
+      </c>
+      <c r="D112" t="s">
+        <v>39</v>
+      </c>
+      <c r="E112" t="s">
+        <v>39</v>
+      </c>
+      <c r="F112" t="s">
+        <v>78</v>
+      </c>
+      <c r="G112">
+        <v>2</v>
+      </c>
+      <c r="H112">
+        <v>1</v>
+      </c>
+      <c r="I112">
+        <v>1</v>
+      </c>
+      <c r="J112">
+        <v>0</v>
+      </c>
+      <c r="L112" s="1">
+        <v>1.2899999999999999E-10</v>
+      </c>
+      <c r="M112">
+        <v>0</v>
+      </c>
+      <c r="N112" s="1">
+        <v>0</v>
+      </c>
+      <c r="O112">
+        <v>0</v>
+      </c>
+      <c r="P112">
+        <v>0</v>
+      </c>
+      <c r="Q112">
+        <v>0</v>
+      </c>
+      <c r="R112">
+        <v>0</v>
+      </c>
+      <c r="S112">
+        <v>0</v>
+      </c>
+      <c r="T112">
+        <v>0</v>
+      </c>
+      <c r="U112">
+        <v>0</v>
+      </c>
+      <c r="V112" t="s">
+        <v>249</v>
+      </c>
+      <c r="W112" t="s">
+        <v>250</v>
+      </c>
+      <c r="X112" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y112" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="257" spans="12:23" x14ac:dyDescent="0.25">
@@ -8896,7 +8999,7 @@
   <dimension ref="A1:AF684"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A368" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A634" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
@@ -53501,8 +53604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -53961,7 +54064,7 @@
         <v>112</v>
       </c>
       <c r="G14" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="V14" t="s">
         <v>243</v>
@@ -53987,9 +54090,113 @@
         <v>112</v>
       </c>
       <c r="G15" t="s">
+        <v>82</v>
+      </c>
+      <c r="V15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>225</v>
+      </c>
+      <c r="B16" t="s">
+        <v>224</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>247</v>
+      </c>
+      <c r="E16" t="s">
+        <v>246</v>
+      </c>
+      <c r="F16" t="s">
         <v>112</v>
       </c>
-      <c r="V15" t="s">
+      <c r="G16" t="s">
+        <v>82</v>
+      </c>
+      <c r="V16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>225</v>
+      </c>
+      <c r="B17" t="s">
+        <v>248</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" t="s">
+        <v>246</v>
+      </c>
+      <c r="F17" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" t="s">
+        <v>82</v>
+      </c>
+      <c r="V17" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B18" t="s">
+        <v>225</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="s">
+        <v>246</v>
+      </c>
+      <c r="F18" t="s">
+        <v>112</v>
+      </c>
+      <c r="G18" t="s">
+        <v>82</v>
+      </c>
+      <c r="V18" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>227</v>
+      </c>
+      <c r="B19" t="s">
+        <v>225</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" t="s">
+        <v>246</v>
+      </c>
+      <c r="F19" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" t="s">
+        <v>82</v>
+      </c>
+      <c r="V19" t="s">
         <v>243</v>
       </c>
     </row>

</xml_diff>